<commit_message>
Citations and tightenting of the article
- revised introduction from Jonathan was incorporated,
- citations were added to cover recent articles in IJMS, expanded literature review and referneces to Olaf Andersen CT-scans, and Brooks Smith micro-simulator work,
- Content was tightented, especially the abstract and conclusions.
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FoamFireArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A3744-BA1C-4A05-ABF2-87E91B8CE473}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3B16B7-9515-4342-A8B5-D225C0EFB719}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6090" yWindow="1398" windowWidth="20640" windowHeight="11520" xr2:uid="{08FBFCE1-0EAA-4365-BB72-9455FEE77550}"/>
+    <workbookView xWindow="0" yWindow="1398" windowWidth="20640" windowHeight="11520" xr2:uid="{08FBFCE1-0EAA-4365-BB72-9455FEE77550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Reviewer</t>
   </si>
@@ -168,12 +168,6 @@
   </si>
   <si>
     <t>Also add reference to MetFoam article by Olaf Andersen.</t>
-  </si>
-  <si>
-    <t>Check Jonathan's changes</t>
-  </si>
-  <si>
-    <t>Check Jonathan work first</t>
   </si>
   <si>
     <t>Figure</t>
@@ -233,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -249,6 +243,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,11 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4C09CC-6689-4FF0-AEA9-E91F38CF48A9}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -632,23 +631,23 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -669,14 +668,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
@@ -687,14 +686,14 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
@@ -705,34 +704,37 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+    <row r="5" spans="1:14" ht="49.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
@@ -743,37 +745,34 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
@@ -785,13 +784,13 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
@@ -801,18 +800,15 @@
         <v>7</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+    </row>
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
@@ -822,11 +818,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11">
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D11" t="s">
@@ -837,13 +834,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+      <c r="A12" s="6">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
@@ -853,35 +850,35 @@
         <v>6</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="6">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="6">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
@@ -890,18 +887,15 @@
       <c r="E14" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
@@ -911,14 +905,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6">
+        <v>3</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
@@ -930,13 +924,13 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D17" t="s">
@@ -947,13 +941,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="A18" s="6">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
@@ -963,17 +957,17 @@
         <v>7</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="6">
+        <v>3</v>
+      </c>
+      <c r="B19" s="6">
         <v>6</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D19" t="s">
@@ -983,17 +977,17 @@
         <v>7</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="6">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6">
         <v>7</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D20" t="s">
@@ -1005,13 +999,13 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="6">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
@@ -1021,17 +1015,17 @@
         <v>6</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="6">
+        <v>3</v>
+      </c>
+      <c r="B22" s="6">
         <v>9</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D22" t="s">
@@ -1041,14 +1035,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="6">
+        <v>3</v>
+      </c>
+      <c r="B23" s="6">
         <v>10</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
@@ -1059,31 +1053,31 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="6">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6">
         <v>11</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6">
         <v>12</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
@@ -1093,14 +1087,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="6">
+        <v>3</v>
+      </c>
+      <c r="B26" s="6">
         <v>13</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
@@ -1111,33 +1105,33 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="6">
+        <v>3</v>
+      </c>
+      <c r="B27" s="6">
         <v>14</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
+      <c r="A28" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28" s="6">
         <v>15</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
@@ -1175,20 +1169,13 @@
       <c r="C39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E28" xr:uid="{A850A427-2AAA-426F-94C7-6E099FDD152B}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="In-progress"/>
-        <filter val="Not-started"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E28" xr:uid="{A850A427-2AAA-426F-94C7-6E099FDD152B}"/>
   <conditionalFormatting sqref="E2">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E28 G7 G9">
+  <conditionalFormatting sqref="E3:E28 G5 G9">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",E3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Moved figures with error bars to TEX-FIGURES
I have removed additional folder with figures with error bars and places all the upadeted Figures in TEX-FIGURES
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ss0052\Dropbox\Praca\Research\Steel Foam\Projects\Fire-Luiz_Miguel\Results\ARTICLE\REVISION\FoamFireArticle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FoamFireArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEC1FED-1D3F-49BE-8963-E0EB421E15B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3B16B7-9515-4342-A8B5-D225C0EFB719}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="22296" windowHeight="13152" xr2:uid="{08FBFCE1-0EAA-4365-BB72-9455FEE77550}"/>
+    <workbookView xWindow="0" yWindow="1398" windowWidth="20640" windowHeight="11520" xr2:uid="{08FBFCE1-0EAA-4365-BB72-9455FEE77550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Reviewer</t>
   </si>
@@ -167,10 +167,13 @@
     <t>Why only two samples per temperature were used?</t>
   </si>
   <si>
-    <t>Because of small COV between the samples and limited number of samples.</t>
-  </si>
-  <si>
     <t>Also add reference to MetFoam article by Olaf Andersen.</t>
+  </si>
+  <si>
+    <t>Figure</t>
+  </si>
+  <si>
+    <t>Citations</t>
   </si>
 </sst>
 </file>
@@ -186,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,7 +198,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,16 +227,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,15 +585,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4C09CC-6689-4FF0-AEA9-E91F38CF48A9}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.1015625" customWidth="1"/>
+    <col min="1" max="1" width="6.734375" customWidth="1"/>
+    <col min="2" max="2" width="5.83984375" customWidth="1"/>
     <col min="3" max="3" width="31.89453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.89453125" customWidth="1"/>
     <col min="5" max="5" width="10.3671875" customWidth="1"/>
@@ -603,20 +631,23 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -637,126 +668,129 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="49.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
@@ -765,15 +799,16 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
@@ -784,10 +819,11 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D11" t="s">
@@ -798,13 +834,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+      <c r="A12" s="6">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
@@ -813,49 +849,53 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
+      <c r="F12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="6">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="6">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
@@ -866,13 +906,13 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="6">
+        <v>3</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
@@ -881,35 +921,33 @@
       <c r="E16" t="s">
         <v>5</v>
       </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="A18" s="6">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
@@ -918,15 +956,18 @@
       <c r="E18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
+      <c r="F18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="6">
+        <v>3</v>
+      </c>
+      <c r="B19" s="6">
         <v>6</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D19" t="s">
@@ -935,15 +976,18 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
+      <c r="F19" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="6">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6">
         <v>7</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D20" t="s">
@@ -952,16 +996,16 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="6">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
@@ -970,16 +1014,18 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="6">
+        <v>3</v>
+      </c>
+      <c r="B22" s="6">
         <v>9</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D22" t="s">
@@ -990,13 +1036,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="6">
+        <v>3</v>
+      </c>
+      <c r="B23" s="6">
         <v>10</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
@@ -1007,30 +1053,31 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="6">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6">
         <v>11</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6">
         <v>12</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
@@ -1041,13 +1088,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="6">
+        <v>3</v>
+      </c>
+      <c r="B26" s="6">
         <v>13</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
@@ -1057,34 +1104,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27">
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="6">
+        <v>3</v>
+      </c>
+      <c r="B27" s="6">
         <v>14</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
+      <c r="A28" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28" s="6">
         <v>15</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
@@ -1093,6 +1140,33 @@
       <c r="E28" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C32"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C33"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C39"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E28" xr:uid="{A850A427-2AAA-426F-94C7-6E099FDD152B}"/>
@@ -1101,7 +1175,7 @@
       <formula>NOT(ISERROR(SEARCH("Completed",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E28 G7">
+  <conditionalFormatting sqref="E3:E28 G5 G9">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",E3)))</formula>
     </cfRule>
@@ -1115,5 +1189,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Fig08a and Fig08b
- also ticked off a few items in Workplan
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FoamFireArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3B16B7-9515-4342-A8B5-D225C0EFB719}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2E3580-2390-4919-82B2-0BE5B8AAC6CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1398" windowWidth="20640" windowHeight="11520" xr2:uid="{08FBFCE1-0EAA-4365-BB72-9455FEE77550}"/>
+    <workbookView xWindow="0" yWindow="312" windowWidth="20778" windowHeight="11916" xr2:uid="{08FBFCE1-0EAA-4365-BB72-9455FEE77550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,12 +208,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -227,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -239,9 +233,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -587,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4C09CC-6689-4FF0-AEA9-E91F38CF48A9}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -631,13 +622,13 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
@@ -669,13 +660,13 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
@@ -687,13 +678,13 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
@@ -705,13 +696,13 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="49.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
@@ -728,13 +719,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
@@ -746,13 +737,13 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D7" t="s">
@@ -766,13 +757,13 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
@@ -784,31 +775,30 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="6">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>2</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
@@ -819,11 +809,11 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D11" t="s">
@@ -834,13 +824,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="5">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
@@ -854,13 +844,13 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>2</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
@@ -872,30 +862,30 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="6">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5">
         <v>1</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="6">
-        <v>3</v>
-      </c>
-      <c r="B15" s="6">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
@@ -906,13 +896,13 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6">
-        <v>3</v>
-      </c>
-      <c r="B16" s="6">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="A16" s="5">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
@@ -924,13 +914,13 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="6">
-        <v>3</v>
-      </c>
-      <c r="B17" s="6">
+      <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
         <v>4</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D17" t="s">
@@ -941,13 +931,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="6">
-        <v>3</v>
-      </c>
-      <c r="B18" s="6">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
@@ -961,13 +951,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="6">
-        <v>3</v>
-      </c>
-      <c r="B19" s="6">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
         <v>6</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D19" t="s">
@@ -981,13 +971,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="6">
-        <v>3</v>
-      </c>
-      <c r="B20" s="6">
+      <c r="A20" s="5">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
         <v>7</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D20" t="s">
@@ -999,33 +989,33 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="6">
-        <v>3</v>
-      </c>
-      <c r="B21" s="6">
-        <v>8</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="5">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="6">
-        <v>3</v>
-      </c>
-      <c r="B22" s="6">
+      <c r="A22" s="5">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5">
         <v>9</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D22" t="s">
@@ -1036,13 +1026,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="6">
-        <v>3</v>
-      </c>
-      <c r="B23" s="6">
+      <c r="A23" s="5">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5">
         <v>10</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
@@ -1053,13 +1043,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="6">
-        <v>3</v>
-      </c>
-      <c r="B24" s="6">
+      <c r="A24" s="5">
+        <v>3</v>
+      </c>
+      <c r="B24" s="5">
         <v>11</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="s">
@@ -1071,13 +1061,13 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="6">
-        <v>3</v>
-      </c>
-      <c r="B25" s="6">
+      <c r="A25" s="5">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5">
         <v>12</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
@@ -1088,13 +1078,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="6">
-        <v>3</v>
-      </c>
-      <c r="B26" s="6">
+      <c r="A26" s="5">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5">
         <v>13</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
@@ -1105,13 +1095,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="6">
-        <v>3</v>
-      </c>
-      <c r="B27" s="6">
+      <c r="A27" s="5">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5">
         <v>14</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D27" t="s">
@@ -1125,13 +1115,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="6">
-        <v>3</v>
-      </c>
-      <c r="B28" s="6">
+      <c r="A28" s="5">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5">
         <v>15</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">

</xml_diff>